<commit_message>
[Feat]: Modificacion de Sucursales y Roles para impresion de excel, actualizacion de archivo excel de reactivos
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/reagent/ReactivoFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/reagent/ReactivoFormulario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAPAXSIS-00\source\repos\LaboratorioRamos\Service.Catalog\wwwroot\layout\excel\reagent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CC1A84-9ECA-4C58-A8AB-BAD5ADDF74F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5C8D4E-CEC1-4945-8CB9-A8229EF1686F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="780" windowWidth="20730" windowHeight="11160" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{3229E258-B22D-4941-8A9E-0DA32DA258DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Reactivos" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
     <t>{{Reactivo.NombreSistema}}</t>
   </si>
   <si>
-    <t>{{Reactivo.ActivoDescripcion}}</t>
+    <t>{{Reactivo.Activo}}</t>
   </si>
 </sst>
 </file>
@@ -179,14 +179,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,7 +560,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,22 +569,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
@@ -592,37 +592,37 @@
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>